<commit_message>
refactered the trading modules' code
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/Trades/LongTrades/GILD/GILDBagTradeLongHold.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/Trades/LongTrades/GILD/GILDBagTradeLongHold.xlsx
@@ -363,9 +363,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -401,25 +403,14 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
       <c r="C2">
         <v>10000</v>
       </c>
       <c r="E2">
         <v>81.7</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>